<commit_message>
Ajout de la tole de stoppage et son maintient
</commit_message>
<xml_diff>
--- a/predim.xlsx
+++ b/predim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DamienCM\Desktop\S8\constru\projet_constru_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7096B8A-BDCB-4C02-A401-8234671C1F91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC76EB3-2114-4EE3-A462-6C2DC51078CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{23E1D9DF-2C04-49B7-A416-EF09900865C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{23E1D9DF-2C04-49B7-A416-EF09900865C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Partie 1" sheetId="1" r:id="rId1"/>
@@ -1289,8 +1289,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="F11" s="7">
         <f>3/2*F9*B13/B12/B14^2</f>
-        <v>79.113950536050837</v>
+        <v>68.125901850488219</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>43</v>
@@ -1557,8 +1557,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="2">
-        <f>2*B11</f>
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>34</v>
@@ -2240,15 +2239,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:H34"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:H24"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:H34"/>
   </mergeCells>
   <conditionalFormatting sqref="F12">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">

</xml_diff>